<commit_message>
complete update of code base
</commit_message>
<xml_diff>
--- a/angular/src/assets/sampleFiles/ImportUsersSampleFile.xlsx
+++ b/angular/src/assets/sampleFiles/ImportUsersSampleFile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emre\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\aspnet-zero-core\angular\src\assets\sampleFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F89B5A6F-2AB7-4DF2-B83C-11ACFD46CB62}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A6772E4-D73D-4965-AB94-A892FD5ACA67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{43AB8392-857F-4ABD-83B0-FE7F14CA1608}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{43AB8392-857F-4ABD-83B0-FE7F14CA1608}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -66,19 +66,19 @@
     <t>jurQ892*</t>
   </si>
   <si>
-    <t>UserName*</t>
-  </si>
-  <si>
-    <t>Name*</t>
-  </si>
-  <si>
-    <t>Surname*</t>
-  </si>
-  <si>
-    <t>EmailAddress*</t>
-  </si>
-  <si>
-    <t>Password*</t>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Surname</t>
+  </si>
+  <si>
+    <t>EmailAddress</t>
+  </si>
+  <si>
+    <t>Password</t>
   </si>
 </sst>
 </file>
@@ -444,21 +444,21 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" customWidth="1"/>
-    <col min="2" max="2" width="20.140625" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="18.453125" customWidth="1"/>
+    <col min="2" max="2" width="20.1796875" customWidth="1"/>
+    <col min="3" max="3" width="14.453125" customWidth="1"/>
     <col min="4" max="4" width="22" customWidth="1"/>
-    <col min="5" max="5" width="26.85546875" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" customWidth="1"/>
-    <col min="7" max="7" width="36.140625" customWidth="1"/>
+    <col min="5" max="5" width="26.81640625" customWidth="1"/>
+    <col min="6" max="6" width="16.81640625" customWidth="1"/>
+    <col min="7" max="7" width="36.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -481,7 +481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -504,7 +504,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -527,7 +527,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D4" s="1"/>
     </row>
   </sheetData>

</xml_diff>